<commit_message>
Protokol mit den Fällen des Servers ergänzt
</commit_message>
<xml_diff>
--- a/Protokol Login.xlsx
+++ b/Protokol Login.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20342"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{868DD72F-CC85-4444-B65C-D011B557F038}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2911D878-ADCA-4391-9BD8-4C1C2938966A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Login erfolgreich</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>Login gescheitert - gebannt</t>
+  </si>
+  <si>
+    <t>Loginversuch - Username Passwort</t>
+  </si>
+  <si>
+    <t>Register - Username Passwort</t>
   </si>
 </sst>
 </file>
@@ -361,7 +367,7 @@
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B2:B3"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -439,10 +445,16 @@
       <c r="A10">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>